<commit_message>
Versão inicial da interface final artefatos
</commit_message>
<xml_diff>
--- a/dados_saida/NotaFiscal_256422787.xlsx
+++ b/dados_saida/NotaFiscal_256422787.xlsx
@@ -518,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5228</t>
+          <t>a7e898</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NÃO INFORMADO</t>
+          <t>não informado</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">

</xml_diff>